<commit_message>
whoisapy with 50 jsons
</commit_message>
<xml_diff>
--- a/EXAMPLE.xlsx
+++ b/EXAMPLE.xlsx
@@ -462,11 +462,11 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>479591</v>
+        <v>830470</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Bolivia, Plurinational State of</t>
+          <t>Norfolk Island</t>
         </is>
       </c>
     </row>
@@ -478,7 +478,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>254142</v>
+        <v>9223</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -494,11 +494,11 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>85669</v>
+        <v>80749</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Bouvet Island</t>
+          <t>Saint Lucia</t>
         </is>
       </c>
     </row>
@@ -510,11 +510,11 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>131570</v>
+        <v>72605</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Czechia</t>
+          <t>Christmas Island</t>
         </is>
       </c>
     </row>
@@ -526,11 +526,11 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>15710</v>
+        <v>734</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Belize</t>
+          <t>Lao People's Democratic Republic</t>
         </is>
       </c>
     </row>
@@ -542,11 +542,11 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>12978</v>
+        <v>1717</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Anguilla</t>
+          <t>Portugal</t>
         </is>
       </c>
     </row>
@@ -558,11 +558,11 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1244</v>
+        <v>1160</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Isle of Man</t>
+          <t>Maldives</t>
         </is>
       </c>
     </row>
@@ -574,11 +574,11 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>6747</v>
+        <v>3061</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Panama</t>
+          <t>Liberia</t>
         </is>
       </c>
     </row>
@@ -590,11 +590,11 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>8850</v>
+        <v>19</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>South Africa</t>
+          <t>Czechia</t>
         </is>
       </c>
     </row>
@@ -606,11 +606,11 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>776</v>
+        <v>190</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Côte d'Ivoire</t>
+          <t>Nicaragua</t>
         </is>
       </c>
     </row>
@@ -622,11 +622,11 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>201</v>
+        <v>54</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Yemen</t>
+          <t>Micronesia, Federated States of</t>
         </is>
       </c>
     </row>
@@ -638,11 +638,11 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1751</v>
+        <v>1</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Tonga</t>
+          <t>Maldives</t>
         </is>
       </c>
     </row>
@@ -654,11 +654,11 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>278</v>
+        <v>0</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Belgium</t>
+          <t>Cuba</t>
         </is>
       </c>
     </row>
@@ -670,11 +670,11 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>124</v>
+        <v>0</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Timor-Leste</t>
+          <t>Guernsey</t>
         </is>
       </c>
     </row>
@@ -686,11 +686,11 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>51</v>
+        <v>0</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Svalbard and Jan Mayen</t>
         </is>
       </c>
     </row>
@@ -702,11 +702,11 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>160</v>
+        <v>0</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Argentina</t>
+          <t>Andorra</t>
         </is>
       </c>
     </row>
@@ -718,11 +718,11 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>158</v>
+        <v>17</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Cayman Islands</t>
+          <t>Palau</t>
         </is>
       </c>
     </row>

</xml_diff>